<commit_message>
Code Merging for NI_FourWeekly A to D
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite WeeklyCatB201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite WeeklyCatB201718.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="84" windowWidth="14340" windowHeight="4452" activeTab="3"/>
+    <workbookView activeTab="3" windowHeight="4452" windowWidth="14340" xWindow="384" yWindow="84"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="NIWeeklyCat_B" sheetId="2" r:id="rId2"/>
-    <sheet name="ProcessPayrollForNIWeekly" sheetId="4" r:id="rId3"/>
-    <sheet name="TestReports" sheetId="5" r:id="rId4"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="NIWeeklyCat_B" r:id="rId2" sheetId="2"/>
+    <sheet name="ProcessPayrollForNIWeekly" r:id="rId3" sheetId="4"/>
+    <sheet name="TestReports" r:id="rId4" sheetId="5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="55">
   <si>
     <t>TC</t>
   </si>
@@ -188,6 +188,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -257,48 +258,48 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -312,10 +313,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -473,7 +474,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -482,13 +483,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -498,7 +499,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -507,7 +508,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -516,7 +517,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -526,12 +527,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -562,7 +563,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -581,7 +582,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -593,7 +594,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -602,10 +603,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -678,7 +679,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -689,7 +690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row ht="57.6" r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -704,13 +705,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -719,10 +720,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="82.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="82.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -748,7 +749,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="21.6" r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -902,12 +903,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -916,19 +917,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.77734375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="53.6640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="52.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.77734375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="53.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="26.4" r="1" s="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>34</v>
       </c>
@@ -969,7 +970,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="8" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="28.8" r="2" s="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>53</v>
       </c>
@@ -1004,7 +1005,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row customFormat="1" ht="28.8" r="3" s="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>53</v>
       </c>
@@ -1039,7 +1040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row customFormat="1" ht="28.8" r="4" s="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>53</v>
       </c>
@@ -1074,7 +1075,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row customFormat="1" ht="28.8" r="5" s="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>53</v>
       </c>
@@ -1109,7 +1110,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row customFormat="1" ht="28.8" r="6" s="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>53</v>
       </c>
@@ -1144,7 +1145,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row customFormat="1" ht="28.8" r="7" s="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>53</v>
       </c>
@@ -1179,7 +1180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row customFormat="1" ht="28.8" r="8" s="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>53</v>
       </c>
@@ -1214,7 +1215,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row customFormat="1" ht="28.8" r="9" s="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>53</v>
       </c>
@@ -1249,7 +1250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row customFormat="1" ht="28.8" r="10" s="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>53</v>
       </c>
@@ -1286,16 +1287,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
-    <hyperlink ref="A3:A10" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId1" ref="A2"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId2" ref="A3:A10"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId3" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1304,19 +1305,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.21875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.21875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="41.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.21875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.77734375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="51.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.21875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="26.21875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="41.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.21875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="26.4" r="1" s="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>34</v>
       </c>
@@ -1360,7 +1361,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="28.8" r="2" s="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>53</v>
       </c>
@@ -1400,8 +1401,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Resetting once again the internal pagination of payroll as per the new automation Org payfrequencies
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite WeeklyCatB201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite WeeklyCatB201718.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="90" windowWidth="14340" windowHeight="4455" activeTab="3"/>
+    <workbookView activeTab="3" windowHeight="4455" windowWidth="14340" xWindow="390" yWindow="90"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="NIWeeklyCat_B" sheetId="2" r:id="rId2"/>
-    <sheet name="ProcessPayrollForNIWeekly" sheetId="4" r:id="rId3"/>
-    <sheet name="TestReports" sheetId="5" r:id="rId4"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="NIWeeklyCat_B" r:id="rId2" sheetId="2"/>
+    <sheet name="ProcessPayrollForNIWeekly" r:id="rId3" sheetId="4"/>
+    <sheet name="TestReports" r:id="rId4" sheetId="5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="54">
   <si>
     <t>TC</t>
   </si>
@@ -190,6 +190,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -259,45 +260,45 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -314,10 +315,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -352,7 +353,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -404,7 +405,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -509,7 +510,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -518,13 +519,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -534,7 +535,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -543,7 +544,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -552,7 +553,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -562,12 +563,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -598,7 +599,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -617,7 +618,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -629,7 +630,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -638,10 +639,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -714,7 +715,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -725,7 +726,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row ht="60" r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -740,13 +741,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -755,10 +756,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="82.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="82.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -784,7 +785,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="21.6" r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>43</v>
       </c>
@@ -938,12 +939,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -952,19 +953,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="53.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="52.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="53.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="26.45" r="1" s="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
@@ -1005,7 +1006,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="8" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="28.9" r="2" s="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>52</v>
       </c>
@@ -1040,7 +1041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="3" s="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>52</v>
       </c>
@@ -1075,7 +1076,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="4" s="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>52</v>
       </c>
@@ -1110,7 +1111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="5" s="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>52</v>
       </c>
@@ -1145,7 +1146,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="6" s="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>52</v>
       </c>
@@ -1180,7 +1181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="7" s="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>52</v>
       </c>
@@ -1215,7 +1216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="8" s="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>52</v>
       </c>
@@ -1250,7 +1251,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="9" s="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>52</v>
       </c>
@@ -1285,7 +1286,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="10" s="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>52</v>
       </c>
@@ -1322,15 +1323,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2:A10" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2:A10"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1339,19 +1340,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="41.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="51.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="41.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="26.45" r="1" s="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
@@ -1395,7 +1396,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="49.5" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>52</v>
       </c>
@@ -1435,8 +1436,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>